<commit_message>
Minor changes in Update processing
</commit_message>
<xml_diff>
--- a/static/hrdata.xlsx
+++ b/static/hrdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212632683\Box Sync\DTLP\HR Chat Bot\GErusHRChatBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Projects\GErusHRChatBot\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -75,16 +75,67 @@
   </si>
   <si>
     <t>Для получения расчетного листа обратитесь в бухгалтерию</t>
+  </si>
+  <si>
+    <t>Карьерные возможности</t>
+  </si>
+  <si>
+    <t>Лидерские программы в ДжиИ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возможности для PB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возможности для LPB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возможности для SPB </t>
+  </si>
+  <si>
+    <t>http://leadershipprograms.ge.com/</t>
+  </si>
+  <si>
+    <t>Bubble Assignment - подключение на временный проект с частичной занятостью и высокой целью. Обращайтесь к вашему менеджеру и HR менеджеру</t>
+  </si>
+  <si>
+    <t>Лидерские программы начального уровня</t>
+  </si>
+  <si>
+    <t>Manager's Academy - обучающая программа для начинающих руководителей. Номинация от бизнеса - обращайтесь к HRM</t>
+  </si>
+  <si>
+    <t>IDP - индивидуальный план развития, прорабатывается совместно с менеджером и HR менеджером</t>
+  </si>
+  <si>
+    <t>Лидерские программы -  XLP</t>
+  </si>
+  <si>
+    <t>Лидерские программы - RISE / XLP</t>
+  </si>
+  <si>
+    <t>STIR - командировка до 3х месяцев за границей с целью обучения, погружения в новые процессы, перенятие опыта. Обращайтесь к HRM</t>
+  </si>
+  <si>
+    <t>Dual role - для смельчаков, готовых взять на себя дополнительные обязанности! Обращайтесь к Вашему HRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -108,13 +159,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,17 +484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,7 +505,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -462,7 +519,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2">
@@ -476,7 +533,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3">
@@ -490,7 +547,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4">
@@ -502,13 +559,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,11 +575,11 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,11 +589,11 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,13 +601,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,13 +615,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,11 +631,11 @@
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,13 +643,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,10 +657,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -614,10 +671,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -628,10 +685,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -642,16 +699,229 @@
         <v>14</v>
       </c>
       <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C30" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>